<commit_message>
- ‘Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.csv’ / ‘Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx’
</commit_message>
<xml_diff>
--- a/Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx
+++ b/Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx
@@ -870,9 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -892,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>13509</v>
+        <v>175.774</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -903,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>72202</v>
+        <v>939.46400000000006</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -914,7 +912,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>45345</v>
+        <v>590.01099999999997</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -925,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>15946</v>
+        <v>207.483</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -936,7 +934,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>37086</v>
+        <v>482.54899999999998</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -947,7 +945,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>17807</v>
+        <v>231.69800000000001</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -958,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>70153</v>
+        <v>912.803</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -969,7 +967,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>20025</v>
+        <v>260.55700000000002</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -980,7 +978,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>15444</v>
+        <v>200.95099999999999</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -991,7 +989,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>21057</v>
+        <v>273.98500000000001</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -1002,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>19118</v>
+        <v>248.756</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -1013,7 +1011,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>18598</v>
+        <v>241.99</v>
       </c>
       <c r="C13">
         <v>100</v>

</xml_diff>

<commit_message>
/ ‘Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx’
</commit_message>
<xml_diff>
--- a/Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx
+++ b/Thesis/Images/Ti-6242/Microstructures/Edited/Ti6242-1.1-CS-5(500x) - Threshold.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Ti6242-1.1-CS-5(500x) - Thresho" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -28,6 +28,18 @@
   </si>
   <si>
     <t>%Area</t>
+  </si>
+  <si>
+    <t>Area - 146.01*116.81</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Area Fraction</t>
   </si>
 </sst>
 </file>
@@ -868,13 +880,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,7 +913,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -906,8 +923,15 @@
       <c r="C3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f>146.01*116.81</f>
+        <v>17055.428100000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -917,8 +941,15 @@
       <c r="C4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f>STDEV(B2:B13)</f>
+        <v>275.55940249491778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -928,8 +959,14 @@
       <c r="C5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>397.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -939,8 +976,15 @@
       <c r="C6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <f>(SUM(B2:B13))*100/F3</f>
+        <v>27.9443058952006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -951,7 +995,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -962,7 +1006,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -973,7 +1017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -984,7 +1028,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -995,7 +1039,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1006,7 +1050,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>